<commit_message>
chore(playground): update invoice example output file
</commit_message>
<xml_diff>
--- a/apps/playground/examples/invoice/output.xlsx
+++ b/apps/playground/examples/invoice/output.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
   <si>
     <t>Name: Playground Invoice</t>
   </si>
@@ -28,10 +28,10 @@
     <t>Price: 12000</t>
   </si>
   <si>
-    <t>Item date: [[items.date]]</t>
-  </si>
-  <si>
-    <t>Missing: [[items.missingProp]]</t>
+    <t>Item date: 2025-01-01</t>
+  </si>
+  <si>
+    <t>Missing: 0</t>
   </si>
   <si>
     <t>ID: 002</t>
@@ -41,6 +41,9 @@
   </si>
   <si>
     <t>Price: 3000</t>
+  </si>
+  <si>
+    <t>Item date: 2025-01-02</t>
   </si>
 </sst>
 </file>
@@ -459,7 +462,7 @@
         <v>9</v>
       </c>
       <c r="D3" t="s">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="E3" t="s">
         <v>6</v>

</xml_diff>